<commit_message>
[Schedule.API] Agregado el modelo de planificacion
</commit_message>
<xml_diff>
--- a/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
+++ b/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Efrain Bastidas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Efrain Bastidas\Desktop\Schedule\Schedule.API\wwwroot\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -426,7 +426,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Agregado el modelo de PlanificacionHorario. Se usara un solo archivo excel con varias "hojas"
</commit_message>
<xml_diff>
--- a/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
+++ b/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PlanificacionAcademica" sheetId="1" r:id="rId1"/>
+    <sheet name="PlanificacionHorarios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ASIGNATURA</t>
   </si>
@@ -47,17 +48,80 @@
     <t>CANT. ALUMNOS</t>
   </si>
   <si>
-    <t>Planificacion Academica Departamento de Ingenieria de Sistemas 20xx-x SEMESTRE XXX</t>
-  </si>
-  <si>
     <t>COD.</t>
+  </si>
+  <si>
+    <t>LUNES</t>
+  </si>
+  <si>
+    <t>MARTES</t>
+  </si>
+  <si>
+    <t>MIERCOLES</t>
+  </si>
+  <si>
+    <t>JUEVES</t>
+  </si>
+  <si>
+    <t>VIERNES</t>
+  </si>
+  <si>
+    <t>SABADO</t>
+  </si>
+  <si>
+    <t>7:00 a 7:50 am</t>
+  </si>
+  <si>
+    <t>7:50 a 8:40 am</t>
+  </si>
+  <si>
+    <t>8:40 a 9:30 am</t>
+  </si>
+  <si>
+    <t>9:30 a 10:20 am</t>
+  </si>
+  <si>
+    <t>10:20 a 11:10 am</t>
+  </si>
+  <si>
+    <t>11:10 a 12:00 am</t>
+  </si>
+  <si>
+    <t>12:00 a 1:00 pm</t>
+  </si>
+  <si>
+    <t>HORA DE ALMUERZO</t>
+  </si>
+  <si>
+    <t>1:00 a 1:50 pm</t>
+  </si>
+  <si>
+    <t>1:50 a 2:40 pm</t>
+  </si>
+  <si>
+    <t>2:40 a 3:30 pm</t>
+  </si>
+  <si>
+    <t>3:30 a 4:20 pm</t>
+  </si>
+  <si>
+    <t>4:20 a 5:10 pm</t>
+  </si>
+  <si>
+    <t>5:10 a 6:00 pm</t>
+  </si>
+  <si>
+    <t>HORARIO DPTO. DE  INGENIERIA DE SISTEMA PERIODO 20xx-x SEMESTRE XXX</t>
+  </si>
+  <si>
+    <t>PLANIFICACION ACADEMICA DEPARTAMENTO DE INGENIERIA DE SISTEMAS PERIODO 20xx-x SEMESTRE XXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +142,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,17 +214,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,33 +572,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -476,4 +632,240 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="9" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregado el modelo de planificacion aulas
</commit_message>
<xml_diff>
--- a/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
+++ b/Schedule.API/wwwroot/Resources/ModeloPlanificacion.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PlanificacionAcademica" sheetId="1" r:id="rId1"/>
     <sheet name="PlanificacionHorarios" sheetId="2" r:id="rId2"/>
+    <sheet name="PlanificacionAulas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>ASIGNATURA</t>
   </si>
@@ -115,6 +116,9 @@
   </si>
   <si>
     <t>PLANIFICACION ACADEMICA DEPARTAMENTO DE INGENIERIA DE SISTEMAS PERIODO 20xx-x SEMESTRE XXX</t>
+  </si>
+  <si>
+    <t>PLANIFICACION AULA XXXX DPTO. DE  INGENIERIA DE SISTEMA PERIODO 20xx-x</t>
   </si>
 </sst>
 </file>
@@ -278,16 +282,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,8 +665,8 @@
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
@@ -755,18 +759,18 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -848,12 +852,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -864,8 +862,242 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="9" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>